<commit_message>
[#130526475] Profile Set (aka Response Set) import now has clearer columns, with a separate one for the slider response and ten choices listed for the multiple choice responses.
</commit_message>
<xml_diff>
--- a/public/profile_sets/imports/Wrapt Response Set Import Template.xlsx
+++ b/public/profile_sets/imports/Wrapt Response Set Import Template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>survey_response_name</t>
   </si>
@@ -22,13 +22,37 @@
     <t>text_response</t>
   </si>
   <si>
-    <t>numeric_response_1</t>
+    <t>slider_response</t>
   </si>
   <si>
-    <t>numeric_response_2</t>
+    <t>choice_1</t>
   </si>
   <si>
-    <t>etc</t>
+    <t>choice_2</t>
+  </si>
+  <si>
+    <t>choice_3</t>
+  </si>
+  <si>
+    <t>choice_4</t>
+  </si>
+  <si>
+    <t>choice_5</t>
+  </si>
+  <si>
+    <t>choice_6</t>
+  </si>
+  <si>
+    <t>choice_7</t>
+  </si>
+  <si>
+    <t>choice_8</t>
+  </si>
+  <si>
+    <t>choice_9</t>
+  </si>
+  <si>
+    <t>choice_10</t>
   </si>
 </sst>
 </file>
@@ -89,7 +113,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="23.43"/>
-    <col customWidth="1" min="4" max="5" width="18.29"/>
+    <col customWidth="1" min="4" max="6" width="18.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -111,6 +135,30 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -119,11 +167,13 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" s="1"/>

</xml_diff>